<commit_message>
Describe what you changed here
</commit_message>
<xml_diff>
--- a/presidents-data/countries.xlsx
+++ b/presidents-data/countries.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacobt/Documents/Linkletter/frontend/presidents-data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacobt/Documents/grid/frontend/presidents-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AF8E676-E2FA-5744-A5A8-3A1594956FA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0899D2A0-EB39-8C4E-97EF-622E448B50AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19560" yWindow="1080" windowWidth="10440" windowHeight="17440" xr2:uid="{CA436EC0-290F-7844-B125-41A799AA7FC0}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{CA436EC0-290F-7844-B125-41A799AA7FC0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1765,8 +1765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D945DC87-F917-344E-801F-B331375726ED}">
   <dimension ref="A1:P197"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N193" zoomScale="98" workbookViewId="0">
-      <selection activeCell="P196" sqref="P196"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="98" workbookViewId="0">
+      <selection activeCell="J41" sqref="J41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>